<commit_message>
LED CocinaB fix v1
</commit_message>
<xml_diff>
--- a/Soft/Dimer.xlsx
+++ b/Soft/Dimer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2.Datos\Electronica\Proyectos\Microchip\Git\Casandra\Soft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9262B3B4-C2AA-4688-8D1C-B63705C4B45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A35B6A0-065A-487E-BDA5-B848F6846371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="486">
   <si>
     <t>Valor</t>
   </si>
@@ -1756,6 +1756,24 @@
   </si>
   <si>
     <t>Comando de encendido de la bomba</t>
+  </si>
+  <si>
+    <t>Reset / Reconect / Exec</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>Estado de Switch Porton</t>
+  </si>
+  <si>
+    <t>Estado de encendido de luz LED</t>
+  </si>
+  <si>
+    <t>Intensidad de encendido de luz LED</t>
+  </si>
+  <si>
+    <t>Modos de encendido del LED</t>
   </si>
 </sst>
 </file>
@@ -2842,7 +2860,7 @@
     <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3442,12 +3460,6 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
@@ -3482,14 +3494,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5163,7 +5175,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A796F4E9-7890-46E8-8DEA-A5685AEE8D14}" name="Tabla1" displayName="Tabla1" ref="A1:H231" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A796F4E9-7890-46E8-8DEA-A5685AEE8D14}" name="Tabla1" displayName="Tabla1" ref="A1:H231" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{37A22C23-BC30-49AA-B326-A1A665DE0E10}" name="N0" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{A945BC43-56EA-42D1-88E7-9CC1375157D6}" name="N1" dataDxfId="6"/>
@@ -8314,8 +8326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D125AF8B-2E62-4DF1-9548-A1621FB537F6}">
   <dimension ref="A1:H231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="H217" sqref="H217"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="F223" sqref="F223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9825,7 +9837,7 @@
       </c>
       <c r="D56" s="180"/>
       <c r="E56" s="29" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="F56" s="25" t="s">
         <v>466</v>
@@ -11524,7 +11536,7 @@
       </c>
       <c r="D119" s="180"/>
       <c r="E119" s="29" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="F119" s="25" t="s">
         <v>465</v>
@@ -12413,7 +12425,7 @@
       </c>
       <c r="D152" s="180"/>
       <c r="E152" s="29" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="F152" s="25" t="s">
         <v>467</v>
@@ -12578,7 +12590,7 @@
         <v>Casandra/Hall/Porton</v>
       </c>
     </row>
-    <row r="159" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="179" t="s">
         <v>53</v>
       </c>
@@ -12603,7 +12615,7 @@
         <v>Casandra/Hall/Timbre</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="182" t="s">
         <v>53</v>
       </c>
@@ -12614,8 +12626,8 @@
         <v>248</v>
       </c>
       <c r="D160" s="183"/>
-      <c r="E160" s="183" t="s">
-        <v>431</v>
+      <c r="E160" s="29" t="s">
+        <v>480</v>
       </c>
       <c r="F160" s="185" t="s">
         <v>468</v>
@@ -12836,7 +12848,7 @@
         <v>Casandra/Caldera/SensorMov/01</v>
       </c>
     </row>
-    <row r="169" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="179" t="s">
         <v>53</v>
       </c>
@@ -12863,7 +12875,7 @@
         <v>Casandra/Caldera/SensorMov/02</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="182" t="s">
         <v>53</v>
       </c>
@@ -12875,7 +12887,7 @@
       </c>
       <c r="D170" s="184"/>
       <c r="E170" s="183" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="F170" s="185" t="s">
         <v>469</v>
@@ -13013,7 +13025,7 @@
         <v>Casandra/Porton/SensPuerta</v>
       </c>
     </row>
-    <row r="176" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="179" t="s">
         <v>53</v>
       </c>
@@ -13038,7 +13050,7 @@
         <v>Casandra/Porton/SensPorton</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="182" t="s">
         <v>53</v>
       </c>
@@ -13049,8 +13061,8 @@
         <v>248</v>
       </c>
       <c r="D177" s="184"/>
-      <c r="E177" s="183" t="s">
-        <v>431</v>
+      <c r="E177" s="29" t="s">
+        <v>480</v>
       </c>
       <c r="F177" s="185" t="s">
         <v>470</v>
@@ -14031,7 +14043,7 @@
       </c>
       <c r="D214" s="29"/>
       <c r="E214" s="29" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="F214" s="25" t="s">
         <v>471</v>
@@ -14069,23 +14081,23 @@
         <v>Casandra/Huerta/On</v>
       </c>
     </row>
-    <row r="216" spans="1:8" s="219" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="B216" s="219" t="s">
+      <c r="B216" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="C216" s="219" t="s">
+      <c r="C216" s="29" t="s">
         <v>427</v>
       </c>
-      <c r="E216" s="219" t="s">
+      <c r="E216" s="29" t="s">
         <v>454</v>
       </c>
-      <c r="F216" s="220" t="s">
+      <c r="F216" s="25" t="s">
         <v>429</v>
       </c>
-      <c r="G216" s="219" t="s">
+      <c r="G216" s="29" t="s">
         <v>307</v>
       </c>
       <c r="H216" s="181" t="str">
@@ -14093,23 +14105,23 @@
         <v>Casandra/Huerta/Off</v>
       </c>
     </row>
-    <row r="217" spans="1:8" s="219" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="B217" s="219" t="s">
+      <c r="B217" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="C217" s="219" t="s">
+      <c r="C217" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="E217" s="219" t="s">
+      <c r="E217" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="F217" s="220" t="s">
+      <c r="F217" s="25" t="s">
         <v>478</v>
       </c>
-      <c r="G217" s="219" t="s">
+      <c r="G217" s="29" t="s">
         <v>307</v>
       </c>
       <c r="H217" s="181" t="str">
@@ -14121,20 +14133,20 @@
       <c r="A218" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="B218" s="219" t="s">
+      <c r="B218" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="C218" s="219" t="s">
+      <c r="C218" s="29" t="s">
         <v>453</v>
       </c>
-      <c r="D218" s="219"/>
-      <c r="E218" s="219" t="s">
+      <c r="D218" s="29"/>
+      <c r="E218" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="F218" s="220" t="s">
+      <c r="F218" s="25" t="s">
         <v>479</v>
       </c>
-      <c r="G218" s="219" t="s">
+      <c r="G218" s="29" t="s">
         <v>307</v>
       </c>
       <c r="H218" s="181" t="str">
@@ -14142,7 +14154,7 @@
         <v>Casandra/Huerta/BbaEstado</v>
       </c>
     </row>
-    <row r="219" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A219" s="182" t="s">
         <v>53</v>
       </c>
@@ -14153,8 +14165,8 @@
         <v>248</v>
       </c>
       <c r="D219" s="183"/>
-      <c r="E219" s="183" t="s">
-        <v>431</v>
+      <c r="E219" s="29" t="s">
+        <v>480</v>
       </c>
       <c r="F219" s="185" t="s">
         <v>472</v>
@@ -14178,8 +14190,12 @@
         <v>476</v>
       </c>
       <c r="D220" s="175"/>
-      <c r="E220" s="175"/>
-      <c r="F220" s="177"/>
+      <c r="E220" s="175" t="s">
+        <v>275</v>
+      </c>
+      <c r="F220" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="G220" s="175" t="s">
         <v>307</v>
       </c>
@@ -14192,16 +14208,20 @@
       <c r="A221" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="B221" s="219" t="s">
+      <c r="B221" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="C221" s="219" t="s">
+      <c r="C221" s="29" t="s">
         <v>474</v>
       </c>
-      <c r="D221" s="219"/>
-      <c r="E221" s="219"/>
-      <c r="F221" s="220"/>
-      <c r="G221" s="219" t="s">
+      <c r="D221" s="29"/>
+      <c r="E221" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="F221" s="25" t="s">
+        <v>484</v>
+      </c>
+      <c r="G221" s="29" t="s">
         <v>307</v>
       </c>
       <c r="H221" s="181" t="str">
@@ -14213,16 +14233,20 @@
       <c r="A222" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="B222" s="219" t="s">
+      <c r="B222" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="C222" s="219" t="s">
+      <c r="C222" s="29" t="s">
         <v>448</v>
       </c>
-      <c r="D222" s="219"/>
-      <c r="E222" s="219"/>
-      <c r="F222" s="220"/>
-      <c r="G222" s="219" t="s">
+      <c r="D222" s="29"/>
+      <c r="E222" s="29" t="s">
+        <v>481</v>
+      </c>
+      <c r="F222" s="25" t="s">
+        <v>485</v>
+      </c>
+      <c r="G222" s="29" t="s">
         <v>307</v>
       </c>
       <c r="H222" s="181" t="str">
@@ -14234,16 +14258,20 @@
       <c r="A223" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="B223" s="219" t="s">
+      <c r="B223" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="C223" s="219" t="s">
+      <c r="C223" s="29" t="s">
         <v>449</v>
       </c>
-      <c r="D223" s="219"/>
-      <c r="E223" s="219"/>
-      <c r="F223" s="220"/>
-      <c r="G223" s="219" t="s">
+      <c r="D223" s="29"/>
+      <c r="E223" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="F223" s="25" t="s">
+        <v>452</v>
+      </c>
+      <c r="G223" s="29" t="s">
         <v>307</v>
       </c>
       <c r="H223" s="181" t="str">
@@ -14255,16 +14283,20 @@
       <c r="A224" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="B224" s="219" t="s">
+      <c r="B224" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="C224" s="219" t="s">
+      <c r="C224" s="29" t="s">
         <v>475</v>
       </c>
-      <c r="D224" s="219"/>
-      <c r="E224" s="219"/>
-      <c r="F224" s="220"/>
-      <c r="G224" s="219" t="s">
+      <c r="D224" s="29"/>
+      <c r="E224" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="F224" s="25" t="s">
+        <v>482</v>
+      </c>
+      <c r="G224" s="29" t="s">
         <v>307</v>
       </c>
       <c r="H224" s="181" t="str">
@@ -14276,16 +14308,20 @@
       <c r="A225" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="B225" s="219" t="s">
+      <c r="B225" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="C225" s="219" t="s">
+      <c r="C225" s="29" t="s">
         <v>318</v>
       </c>
-      <c r="D225" s="219"/>
-      <c r="E225" s="219"/>
-      <c r="F225" s="220"/>
-      <c r="G225" s="219" t="s">
+      <c r="D225" s="29"/>
+      <c r="E225" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="F225" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="G225" s="29" t="s">
         <v>307</v>
       </c>
       <c r="H225" s="181" t="str">
@@ -14305,7 +14341,7 @@
       </c>
       <c r="D226" s="183"/>
       <c r="E226" s="183" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="F226" s="185" t="s">
         <v>473</v>

</xml_diff>